<commit_message>
data/ - Se agrega la columna acronym en el excell y en el python para el Tproject
</commit_message>
<xml_diff>
--- a/data/projectsWEB.xlsx
+++ b/data/projectsWEB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">piproject</t>
   </si>
   <si>
+    <t xml:space="preserve">acronym</t>
+  </si>
+  <si>
     <t xml:space="preserve">nameProject</t>
   </si>
   <si>
@@ -88,7 +91,10 @@
     <t xml:space="preserve">Rocío Pérez-Portela &amp; José Carlos Hernández</t>
   </si>
   <si>
-    <t xml:space="preserve">Genomic divergence, plasticity and microbiome shifts in marine invertebrates along natural environmental gradients (ENVIOME)</t>
+    <t xml:space="preserve">ENVIOME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genomic divergence, plasticity and microbiome shifts in marine invertebrates along natural environmental gradients</t>
   </si>
   <si>
     <t xml:space="preserve">PID2021-128094NB-I00</t>
@@ -132,7 +138,10 @@
     <t xml:space="preserve">logo_enviome2</t>
   </si>
   <si>
-    <t xml:space="preserve">Intraspecific and interspecific biological processes underpinning the adaptability of marine invertebrates to ocean acidification (ACIDOMIC)</t>
+    <t xml:space="preserve">ACIDOMIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intraspecific and interspecific biological processes underpinning the adaptability of marine invertebrates to ocean acidification</t>
   </si>
   <si>
     <t xml:space="preserve">CNS2022-135968</t>
@@ -176,10 +185,10 @@
     <t xml:space="preserve">paracentrotus_Rocío</t>
   </si>
   <si>
-    <t xml:space="preserve">Adaptabilidad genética de las especies marinas en gradientes naturales análogos a los océanos del futuro (DIVERGEN)</t>
-  </si>
-  <si>
     <t xml:space="preserve">DIVERGEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adaptabilidad genética de las especies marinas en gradientes naturales análogos a los océanos del futuro</t>
   </si>
   <si>
     <t xml:space="preserve">07-01-2022</t>
@@ -210,7 +219,10 @@
     <t xml:space="preserve">C. Avila &amp; E.Ballesté</t>
   </si>
   <si>
-    <t xml:space="preserve">HUMAN PRESSURES AND NATURAL HAZARDS: CHALLENGES FOR ANTARCTIC MARINE ECOSYSTEMS (CHALLENGE-2)</t>
+    <t xml:space="preserve">CHALLENGE-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human Pressures and Natural Hazards: Challenges for Antarctic Marine Ecosystems</t>
   </si>
   <si>
     <t xml:space="preserve">PID2022-141628NB-I00/ANT</t>
@@ -236,6 +248,9 @@
   </si>
   <si>
     <t xml:space="preserve">logo_CHALLENGE2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHALLENGE2_MICINN</t>
   </si>
 </sst>
 </file>
@@ -548,7 +563,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -568,7 +583,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -592,7 +607,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -616,10 +631,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -628,6 +639,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -645,11 +660,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -754,23 +769,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:O5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:P5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="16">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="email"/>
     <tableColumn id="3" name="researcher"/>
     <tableColumn id="4" name="piproject"/>
-    <tableColumn id="5" name="nameProject"/>
-    <tableColumn id="6" name="projectID"/>
-    <tableColumn id="7" name="start"/>
-    <tableColumn id="8" name="end"/>
-    <tableColumn id="9" name="summary"/>
-    <tableColumn id="10" name="websiteProject"/>
-    <tableColumn id="11" name="fundingAgency"/>
-    <tableColumn id="12" name="socialNetwork_x"/>
-    <tableColumn id="13" name="socialNetwork_bsky"/>
-    <tableColumn id="14" name="socialNetwork_inst"/>
-    <tableColumn id="15" name="imageID_logo"/>
+    <tableColumn id="5" name="acronym"/>
+    <tableColumn id="6" name="nameProject"/>
+    <tableColumn id="7" name="projectID"/>
+    <tableColumn id="8" name="start"/>
+    <tableColumn id="9" name="end"/>
+    <tableColumn id="10" name="summary"/>
+    <tableColumn id="11" name="websiteProject"/>
+    <tableColumn id="12" name="fundingAgency"/>
+    <tableColumn id="13" name="socialNetwork_x"/>
+    <tableColumn id="14" name="socialNetwork_bsky"/>
+    <tableColumn id="15" name="socialNetwork_inst"/>
+    <tableColumn id="16" name="imageID_logo"/>
   </tableColumns>
 </table>
 </file>
@@ -952,12 +968,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -966,17 +982,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="37.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="132.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="25.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="33.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="27.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="25.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="17" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="37.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="132.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="22.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="33.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="27.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="25.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="18" style="1" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,19 +1008,19 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -1022,7 +1038,7 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="6" t="s">
@@ -1037,184 +1053,220 @@
       <c r="S1" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
     </row>
     <row r="2" s="12" customFormat="true" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>24</v>
       </c>
+      <c r="G2" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="H2" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="J2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="13"/>
+      <c r="L2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="N2" s="13"/>
-      <c r="O2" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="O2" s="13"/>
+      <c r="P2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
     </row>
     <row r="3" s="12" customFormat="true" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="0"/>
+      <c r="X3" s="0"/>
+      <c r="Y3" s="0"/>
+      <c r="Z3" s="0"/>
     </row>
     <row r="4" s="12" customFormat="true" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="I4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="13"/>
+      <c r="L4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="N4" s="13"/>
-      <c r="O4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>46</v>
-      </c>
+      <c r="O4" s="13"/>
+      <c r="P4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
     </row>
     <row r="5" s="12" customFormat="true" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="E5" s="24" t="s">
         <v>53</v>
       </c>
+      <c r="F5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>56</v>
+      </c>
       <c r="I5" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>58</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="M5" s="27"/>
+        <v>59</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>60</v>
+      </c>
       <c r="N5" s="27"/>
-      <c r="O5" s="12" t="s">
-        <v>57</v>
-      </c>
+      <c r="O5" s="27"/>
       <c r="P5" s="12" t="s">
-        <v>56</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>